<commit_message>
Updated manual count feature _38; updated the f-score excel table
</commit_message>
<xml_diff>
--- a/Feature_coding_accuracies_flair_Assignment_Updated.xlsx
+++ b/Feature_coding_accuracies_flair_Assignment_Updated.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahle\Documents\GitHub\Reddit_MDA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tos\Documents\GitHub\Reddit_MDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7730F97-7986-4059-8AD3-C0BC88A660E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8084E4B1-192B-4797-9246-26050B5BE3C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10718" yWindow="0" windowWidth="10965" windowHeight="13763" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feature_coding_accuracies_flair" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="117">
   <si>
     <t>Feature</t>
   </si>
@@ -343,12 +343,6 @@
     <t>Our list of copular verbs to distinguish predicative from attributive did not include contracted forms ("I'm pretty"), added these. Some cases that are not identified are due to interjections and insertions ("You are, in fact, smart") which we can't really control for.</t>
   </si>
   <si>
-    <t>This is being compiled with the exact code in two functions analyze_particle and analyze_adverb. Could this be causing the problem?</t>
-  </si>
-  <si>
-    <t>line 972: we should not have s-copy() there but another dictionary (or another function nested into it)</t>
-  </si>
-  <si>
     <t xml:space="preserve">probably the same problem as "hashtag_201" </t>
   </si>
   <si>
@@ -377,6 +371,15 @@
   </si>
   <si>
     <t>GK (HM)</t>
+  </si>
+  <si>
+    <t>Corrected a few mistakes in the manual coding. Part of it should work once the analyise_function is fixed. We will consider adding "while" and "since" with their specifications after the re-run of the code</t>
+  </si>
+  <si>
+    <t>I don't see a reason why this is not returning positives because the code is simply checking if item is in the  discpart list</t>
+  </si>
+  <si>
+    <t>Axel fixed the problem with the s-copy()</t>
   </si>
 </sst>
 </file>
@@ -873,48 +876,48 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Akzent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Akzent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Akzent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Akzent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Akzent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Akzent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Ausgabe" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Berechnung" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Eingabe" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Überschrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Verknüpfte Zelle" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -930,7 +933,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1228,18 +1231,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K82"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J6" sqref="J6"/>
+      <selection pane="bottomLeft" activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.46484375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="20.1796875" customWidth="1"/>
-    <col min="11" max="11" width="53.36328125" customWidth="1"/>
+    <col min="1" max="1" width="20.19921875" customWidth="1"/>
+    <col min="11" max="11" width="53.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1274,7 +1277,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>73</v>
       </c>
@@ -1303,10 +1306,10 @@
         <v>0.14285714285714199</v>
       </c>
       <c r="J2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -1335,10 +1338,10 @@
         <v>0.4</v>
       </c>
       <c r="J3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>41</v>
       </c>
@@ -1367,10 +1370,10 @@
         <v>0.5</v>
       </c>
       <c r="J4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1399,10 +1402,10 @@
         <v>0.6</v>
       </c>
       <c r="J5" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>77</v>
       </c>
@@ -1434,7 +1437,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>78</v>
       </c>
@@ -1466,7 +1469,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>79</v>
       </c>
@@ -1498,7 +1501,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A9" s="2" t="s">
         <v>83</v>
       </c>
@@ -1533,7 +1536,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>52</v>
       </c>
@@ -1568,7 +1571,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>23</v>
       </c>
@@ -1600,10 +1603,10 @@
         <v>91</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -1638,7 +1641,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>30</v>
       </c>
@@ -1670,10 +1673,10 @@
         <v>91</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>20</v>
       </c>
@@ -1708,7 +1711,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>22</v>
       </c>
@@ -1743,7 +1746,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A16" s="2" t="s">
         <v>24</v>
       </c>
@@ -1775,10 +1778,10 @@
         <v>91</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A17" s="2" t="s">
         <v>84</v>
       </c>
@@ -1810,10 +1813,10 @@
         <v>91</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>89</v>
       </c>
@@ -1848,7 +1851,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -1880,7 +1883,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>43</v>
       </c>
@@ -1912,7 +1915,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>80</v>
       </c>
@@ -1944,7 +1947,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>32</v>
       </c>
@@ -1976,7 +1979,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>33</v>
       </c>
@@ -2008,7 +2011,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>34</v>
       </c>
@@ -2040,7 +2043,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>81</v>
       </c>
@@ -2072,7 +2075,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>82</v>
       </c>
@@ -2104,10 +2107,10 @@
         <v>92</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -2139,7 +2142,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>45</v>
       </c>
@@ -2171,7 +2174,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>59</v>
       </c>
@@ -2203,7 +2206,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>69</v>
       </c>
@@ -2235,7 +2238,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -2267,7 +2270,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>49</v>
       </c>
@@ -2298,8 +2301,11 @@
       <c r="J32" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K32" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>58</v>
       </c>
@@ -2331,10 +2337,10 @@
         <v>94</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>76</v>
       </c>
@@ -2365,11 +2371,11 @@
       <c r="J34" t="s">
         <v>94</v>
       </c>
-      <c r="K34" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K34" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>56</v>
       </c>
@@ -2401,7 +2407,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>68</v>
       </c>
@@ -2433,10 +2439,10 @@
         <v>93</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>72</v>
       </c>
@@ -2468,10 +2474,10 @@
         <v>93</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>39</v>
       </c>
@@ -2503,10 +2509,10 @@
         <v>93</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>40</v>
       </c>
@@ -2538,10 +2544,10 @@
         <v>93</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>37</v>
       </c>
@@ -2573,7 +2579,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>44</v>
       </c>
@@ -2605,7 +2611,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>48</v>
       </c>
@@ -2637,7 +2643,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>35</v>
       </c>
@@ -2666,7 +2672,7 @@
         <v>0.66666666666666596</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -2695,7 +2701,7 @@
         <v>0.66666666666666596</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>70</v>
       </c>
@@ -2724,7 +2730,7 @@
         <v>0.66666666666666596</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>85</v>
       </c>
@@ -2753,7 +2759,7 @@
         <v>0.68965517241379304</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>54</v>
       </c>
@@ -2782,7 +2788,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>25</v>
       </c>
@@ -2811,7 +2817,7 @@
         <v>0.71428571428571397</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>9</v>
       </c>
@@ -2840,7 +2846,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>87</v>
       </c>
@@ -2869,7 +2875,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>86</v>
       </c>
@@ -2898,7 +2904,7 @@
         <v>0.76923076923076905</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -2927,7 +2933,7 @@
         <v>0.79120879120879095</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>15</v>
       </c>
@@ -2956,7 +2962,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>47</v>
       </c>
@@ -2985,7 +2991,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>88</v>
       </c>
@@ -3014,7 +3020,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>28</v>
       </c>
@@ -3043,7 +3049,7 @@
         <v>0.81818181818181801</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>55</v>
       </c>
@@ -3072,7 +3078,7 @@
         <v>0.81818181818181801</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>61</v>
       </c>
@@ -3101,7 +3107,7 @@
         <v>0.81818181818181801</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>74</v>
       </c>
@@ -3130,7 +3136,7 @@
         <v>0.82352941176470495</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
         <v>10</v>
       </c>
@@ -3159,7 +3165,7 @@
         <v>0.83333333333333304</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
         <v>71</v>
       </c>
@@ -3188,7 +3194,7 @@
         <v>0.85714285714285698</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
         <v>90</v>
       </c>
@@ -3217,7 +3223,7 @@
         <v>0.85714285714285698</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
         <v>50</v>
       </c>
@@ -3246,7 +3252,7 @@
         <v>0.86538461538461497</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
         <v>53</v>
       </c>
@@ -3275,7 +3281,7 @@
         <v>0.86842105263157798</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>57</v>
       </c>
@@ -3304,7 +3310,7 @@
         <v>0.86956521739130399</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
         <v>12</v>
       </c>
@@ -3333,7 +3339,7 @@
         <v>0.88721804511278102</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
         <v>46</v>
       </c>
@@ -3362,7 +3368,7 @@
         <v>0.88888888888888895</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>60</v>
       </c>
@@ -3391,7 +3397,7 @@
         <v>0.89655172413793105</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
         <v>14</v>
       </c>
@@ -3420,7 +3426,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
         <v>64</v>
       </c>
@@ -3449,7 +3455,7 @@
         <v>0.93333333333333302</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
         <v>75</v>
       </c>
@@ -3478,7 +3484,7 @@
         <v>0.93333333333333302</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
         <v>31</v>
       </c>
@@ -3507,7 +3513,7 @@
         <v>0.94736842105263097</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
         <v>62</v>
       </c>
@@ -3536,7 +3542,7 @@
         <v>0.952380952380952</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
         <v>63</v>
       </c>
@@ -3565,7 +3571,7 @@
         <v>0.952380952380952</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
         <v>65</v>
       </c>
@@ -3594,7 +3600,7 @@
         <v>0.952380952380952</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
         <v>67</v>
       </c>
@@ -3623,7 +3629,7 @@
         <v>0.952380952380952</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
         <v>16</v>
       </c>
@@ -3652,7 +3658,7 @@
         <v>0.96428571428571397</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
         <v>19</v>
       </c>
@@ -3681,7 +3687,7 @@
         <v>0.967741935483871</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
         <v>17</v>
       </c>
@@ -3710,7 +3716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
         <v>18</v>
       </c>
@@ -3739,7 +3745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
         <v>27</v>
       </c>
@@ -3768,7 +3774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
         <v>66</v>
       </c>

</xml_diff>

<commit_message>
updated manually coded feature _051; updated overview table
</commit_message>
<xml_diff>
--- a/Feature_coding_accuracies_flair_Assignment_Updated.xlsx
+++ b/Feature_coding_accuracies_flair_Assignment_Updated.xlsx
@@ -8,28 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tos\Documents\GitHub\Reddit_MDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8084E4B1-192B-4797-9246-26050B5BE3C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{868E6E0E-D097-4898-8279-D668107752EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10718" yWindow="0" windowWidth="10965" windowHeight="13763" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feature_coding_accuracies_flair" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="118">
   <si>
     <t>Feature</t>
   </si>
@@ -380,6 +371,9 @@
   </si>
   <si>
     <t>Axel fixed the problem with the s-copy()</t>
+  </si>
+  <si>
+    <t>Corrected some mistakes in the manual coding. We should consider specifying [index+1][0] == VB (so when any verb comes after the det) as a pronoun because many of the dscrepancies between human/machine have that in common</t>
   </si>
 </sst>
 </file>
@@ -1231,9 +1225,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K31" sqref="K31"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A30" sqref="A30:XFD30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.46484375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2205,6 +2199,9 @@
       <c r="J29" t="s">
         <v>94</v>
       </c>
+      <c r="K29" s="1" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A30" t="s">

</xml_diff>

<commit_message>
Worked on two features
</commit_message>
<xml_diff>
--- a/Feature_coding_accuracies_flair_Assignment_Updated.xlsx
+++ b/Feature_coding_accuracies_flair_Assignment_Updated.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tos\Documents\GitHub\Reddit_MDA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahle\Documents\GitHub\Reddit_MDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{868E6E0E-D097-4898-8279-D668107752EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA81B64D-807C-43DF-B516-5FBCA3A7E563}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="0" windowWidth="17830" windowHeight="5560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feature_coding_accuracies_flair" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="120">
   <si>
     <t>Feature</t>
   </si>
@@ -322,9 +335,6 @@
     <t>The words in question seem to be tagged as NN most of the time, so I copied the code for finding them into the Noun-section as well.</t>
   </si>
   <si>
-    <t>Not found because sentence-final punctuation is apparently deleted at some point in our code. Can we simple delete the command in line 78? (sentence.strip(string.punctuation))</t>
-  </si>
-  <si>
     <t>Added a missing comma in line 186, but apart from that I can see no reason why these shouldn't be identified. Is there anything wrong with the object "words"? (line 173) - maybe the split-command?</t>
   </si>
   <si>
@@ -374,13 +384,22 @@
   </si>
   <si>
     <t>Corrected some mistakes in the manual coding. We should consider specifying [index+1][0] == VB (so when any verb comes after the det) as a pronoun because many of the dscrepancies between human/machine have that in common</t>
+  </si>
+  <si>
+    <t>This result is probably due to the mistake in the "analyse_sentence" function and will correc itself.</t>
+  </si>
+  <si>
+    <t>It seems like we are counting some conditions twice? E.g. followed by conjuncts inline 778 and line 787. This leads to at least one mistake. But most instances that are missed by the programmes are instances that we are not looking for and that are difficult to look for. What I am confused by are the cases where there is no "and" in the surface form but the programme is still counting them. According to the code surface presence of "and" is a requirement in all cases.</t>
+  </si>
+  <si>
+    <t>A few instances of present participle clauses used in nominal or modifying function instead of adverbial - we have no chance of sorting these out automatically. Corrected 1 mistake in the manual coding. We could consider adding cases where the present participle is directly preceded by "when", "while", "although", "with", or "without" - but Biber probably only means clauses without these subordinators. In this case: correct manual count again!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -518,6 +537,12 @@
     <font>
       <sz val="11"/>
       <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -864,54 +889,55 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Akzent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Akzent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Akzent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Akzent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Akzent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Akzent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Ausgabe" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Berechnung" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Eingabe" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Überschrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Verknüpfte Zelle" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -927,7 +953,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1226,17 +1252,17 @@
   <dimension ref="A1:K82"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A30" sqref="A30:XFD30"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.46484375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.19921875" customWidth="1"/>
-    <col min="11" max="11" width="53.33203125" customWidth="1"/>
+    <col min="1" max="1" width="20.1796875" customWidth="1"/>
+    <col min="11" max="11" width="53.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1271,71 +1297,77 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>0.935828877005347</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2">
         <v>3</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="2">
         <v>174</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="2">
         <v>9</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="2">
         <v>0.25</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="2">
         <v>0.1</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="2">
         <v>0.14285714285714199</v>
       </c>
-      <c r="J2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
+      <c r="J2" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <v>0.98068669527897001</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>3</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="2">
         <v>2</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="2">
         <v>454</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="2">
         <v>7</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="2">
         <v>0.6</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="2">
         <v>0.3</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="2">
         <v>0.4</v>
       </c>
-      <c r="J3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="J3" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>41</v>
       </c>
@@ -1364,10 +1396,10 @@
         <v>0.5</v>
       </c>
       <c r="J4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1396,10 +1428,10 @@
         <v>0.6</v>
       </c>
       <c r="J5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>77</v>
       </c>
@@ -1430,8 +1462,11 @@
       <c r="J6" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="K6" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>78</v>
       </c>
@@ -1462,8 +1497,11 @@
       <c r="J7" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="K7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>79</v>
       </c>
@@ -1494,43 +1532,46 @@
       <c r="J8" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="2" t="s">
+      <c r="K8" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="3">
         <v>0.90291262135922301</v>
       </c>
-      <c r="C9" s="2">
-        <v>0</v>
-      </c>
-      <c r="D9" s="2">
-        <v>0</v>
-      </c>
-      <c r="E9" s="2">
+      <c r="C9" s="3">
+        <v>0</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0</v>
+      </c>
+      <c r="E9" s="3">
         <v>93</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="3">
         <v>10</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J9" s="2" t="s">
+      <c r="G9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J9" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="K9" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="K9" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>52</v>
       </c>
@@ -1562,10 +1603,10 @@
         <v>91</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>23</v>
       </c>
@@ -1597,10 +1638,10 @@
         <v>91</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.45">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -1632,10 +1673,10 @@
         <v>91</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>30</v>
       </c>
@@ -1667,10 +1708,10 @@
         <v>91</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.45">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>20</v>
       </c>
@@ -1705,7 +1746,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>22</v>
       </c>
@@ -1740,7 +1781,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>24</v>
       </c>
@@ -1772,10 +1813,10 @@
         <v>91</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.45">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>84</v>
       </c>
@@ -1807,10 +1848,10 @@
         <v>91</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.45">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>89</v>
       </c>
@@ -1842,10 +1883,10 @@
         <v>91</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -1877,7 +1918,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>43</v>
       </c>
@@ -1909,7 +1950,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>80</v>
       </c>
@@ -1941,7 +1982,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>32</v>
       </c>
@@ -1973,7 +2014,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>33</v>
       </c>
@@ -2005,7 +2046,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>34</v>
       </c>
@@ -2037,7 +2078,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>81</v>
       </c>
@@ -2069,7 +2110,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>82</v>
       </c>
@@ -2101,10 +2142,10 @@
         <v>92</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -2136,7 +2177,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>45</v>
       </c>
@@ -2168,7 +2209,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>59</v>
       </c>
@@ -2200,10 +2241,10 @@
         <v>94</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>69</v>
       </c>
@@ -2235,7 +2276,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -2267,7 +2308,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>49</v>
       </c>
@@ -2299,10 +2340,10 @@
         <v>94</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>58</v>
       </c>
@@ -2334,10 +2375,10 @@
         <v>94</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>76</v>
       </c>
@@ -2369,10 +2410,10 @@
         <v>94</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>56</v>
       </c>
@@ -2404,7 +2445,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>68</v>
       </c>
@@ -2436,10 +2477,10 @@
         <v>93</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>72</v>
       </c>
@@ -2471,10 +2512,10 @@
         <v>93</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>39</v>
       </c>
@@ -2506,10 +2547,10 @@
         <v>93</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>40</v>
       </c>
@@ -2541,10 +2582,10 @@
         <v>93</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>37</v>
       </c>
@@ -2576,7 +2617,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>44</v>
       </c>
@@ -2608,7 +2649,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>48</v>
       </c>
@@ -2640,7 +2681,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>35</v>
       </c>
@@ -2669,7 +2710,7 @@
         <v>0.66666666666666596</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -2698,7 +2739,7 @@
         <v>0.66666666666666596</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>70</v>
       </c>
@@ -2727,7 +2768,7 @@
         <v>0.66666666666666596</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>85</v>
       </c>
@@ -2756,7 +2797,7 @@
         <v>0.68965517241379304</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>54</v>
       </c>
@@ -2785,7 +2826,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>25</v>
       </c>
@@ -2814,7 +2855,7 @@
         <v>0.71428571428571397</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>9</v>
       </c>
@@ -2843,7 +2884,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>87</v>
       </c>
@@ -2872,7 +2913,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>86</v>
       </c>
@@ -2901,7 +2942,7 @@
         <v>0.76923076923076905</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -2930,7 +2971,7 @@
         <v>0.79120879120879095</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>15</v>
       </c>
@@ -2959,7 +3000,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>47</v>
       </c>
@@ -2988,7 +3029,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>88</v>
       </c>
@@ -3017,7 +3058,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>28</v>
       </c>
@@ -3046,7 +3087,7 @@
         <v>0.81818181818181801</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>55</v>
       </c>
@@ -3075,7 +3116,7 @@
         <v>0.81818181818181801</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>61</v>
       </c>
@@ -3104,7 +3145,7 @@
         <v>0.81818181818181801</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>74</v>
       </c>
@@ -3133,7 +3174,7 @@
         <v>0.82352941176470495</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>10</v>
       </c>
@@ -3162,7 +3203,7 @@
         <v>0.83333333333333304</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>71</v>
       </c>
@@ -3191,7 +3232,7 @@
         <v>0.85714285714285698</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>90</v>
       </c>
@@ -3220,7 +3261,7 @@
         <v>0.85714285714285698</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>50</v>
       </c>
@@ -3249,7 +3290,7 @@
         <v>0.86538461538461497</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>53</v>
       </c>
@@ -3278,7 +3319,7 @@
         <v>0.86842105263157798</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>57</v>
       </c>
@@ -3307,7 +3348,7 @@
         <v>0.86956521739130399</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>12</v>
       </c>
@@ -3336,7 +3377,7 @@
         <v>0.88721804511278102</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>46</v>
       </c>
@@ -3365,7 +3406,7 @@
         <v>0.88888888888888895</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>60</v>
       </c>
@@ -3394,7 +3435,7 @@
         <v>0.89655172413793105</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>14</v>
       </c>
@@ -3423,7 +3464,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>64</v>
       </c>
@@ -3452,7 +3493,7 @@
         <v>0.93333333333333302</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>75</v>
       </c>
@@ -3481,7 +3522,7 @@
         <v>0.93333333333333302</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>31</v>
       </c>
@@ -3510,7 +3551,7 @@
         <v>0.94736842105263097</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>62</v>
       </c>
@@ -3539,7 +3580,7 @@
         <v>0.952380952380952</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>63</v>
       </c>
@@ -3568,7 +3609,7 @@
         <v>0.952380952380952</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>65</v>
       </c>
@@ -3597,7 +3638,7 @@
         <v>0.952380952380952</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>67</v>
       </c>
@@ -3626,7 +3667,7 @@
         <v>0.952380952380952</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>16</v>
       </c>
@@ -3655,7 +3696,7 @@
         <v>0.96428571428571397</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>19</v>
       </c>
@@ -3684,7 +3725,7 @@
         <v>0.967741935483871</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>17</v>
       </c>
@@ -3713,7 +3754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>18</v>
       </c>
@@ -3742,7 +3783,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>27</v>
       </c>
@@ -3771,7 +3812,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>66</v>
       </c>

</xml_diff>

<commit_message>
corrected manual coding for two features
</commit_message>
<xml_diff>
--- a/Feature_coding_accuracies_flair_Assignment_Updated.xlsx
+++ b/Feature_coding_accuracies_flair_Assignment_Updated.xlsx
@@ -1,39 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahle\Documents\GitHub\Reddit_MDA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tos\Documents\GitHub\Reddit_MDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA81B64D-807C-43DF-B516-5FBCA3A7E563}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C51C91F2-9964-4AFF-A4F2-7AE751C4E32B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="0" windowWidth="17830" windowHeight="5560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="14235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feature_coding_accuracies_flair" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="124">
   <si>
     <t>Feature</t>
   </si>
@@ -393,13 +380,25 @@
   </si>
   <si>
     <t>A few instances of present participle clauses used in nominal or modifying function instead of adverbial - we have no chance of sorting these out automatically. Corrected 1 mistake in the manual coding. We could consider adding cases where the present participle is directly preceded by "when", "while", "although", "with", or "without" - but Biber probably only means clauses without these subordinators. In this case: correct manual count again!</t>
+  </si>
+  <si>
+    <t>Corrected manual coding; changing code to account for cases with "which" starts the clause ("Which is why we will be sending *our* military forces their way.")</t>
+  </si>
+  <si>
+    <t>Corrected manual coding and changed the code with Axel to account for passiveby in questions</t>
+  </si>
+  <si>
+    <t>Corrected manual coding; changing code: remove "that" and "like" so they don't count as prepositions?</t>
+  </si>
+  <si>
+    <t>Still working on it</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -543,6 +542,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF92D050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -889,55 +895,56 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Akzent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Akzent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Akzent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Akzent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Akzent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Akzent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Ausgabe" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Berechnung" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Eingabe" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Überschrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Verknüpfte Zelle" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -953,7 +960,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1251,18 +1258,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K82"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.46484375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="20.1796875" customWidth="1"/>
-    <col min="11" max="11" width="53.36328125" customWidth="1"/>
+    <col min="1" max="1" width="20.19921875" customWidth="1"/>
+    <col min="3" max="3" width="4.265625" customWidth="1"/>
+    <col min="4" max="4" width="4.06640625" customWidth="1"/>
+    <col min="5" max="5" width="6.9296875" customWidth="1"/>
+    <col min="6" max="6" width="5.1328125" customWidth="1"/>
+    <col min="11" max="11" width="53.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1297,7 +1308,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>73</v>
       </c>
@@ -1332,7 +1343,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>36</v>
       </c>
@@ -1367,7 +1378,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>41</v>
       </c>
@@ -1399,7 +1410,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1431,7 +1442,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>77</v>
       </c>
@@ -1466,7 +1477,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>78</v>
       </c>
@@ -1501,7 +1512,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>79</v>
       </c>
@@ -1536,7 +1547,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
         <v>83</v>
       </c>
@@ -1571,7 +1582,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>52</v>
       </c>
@@ -1606,7 +1617,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>23</v>
       </c>
@@ -1641,7 +1652,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="12" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -1676,7 +1687,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>30</v>
       </c>
@@ -1711,7 +1722,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="14" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>20</v>
       </c>
@@ -1746,7 +1757,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>22</v>
       </c>
@@ -1781,7 +1792,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A16" s="2" t="s">
         <v>24</v>
       </c>
@@ -1816,7 +1827,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="17" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A17" s="2" t="s">
         <v>84</v>
       </c>
@@ -1851,7 +1862,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="18" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>89</v>
       </c>
@@ -1886,7 +1897,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -1918,7 +1929,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>43</v>
       </c>
@@ -1950,7 +1961,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>80</v>
       </c>
@@ -1982,7 +1993,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>32</v>
       </c>
@@ -2014,7 +2025,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>33</v>
       </c>
@@ -2046,7 +2057,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>34</v>
       </c>
@@ -2078,7 +2089,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>81</v>
       </c>
@@ -2110,7 +2121,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>82</v>
       </c>
@@ -2145,7 +2156,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -2176,8 +2187,11 @@
       <c r="J27" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K27" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>45</v>
       </c>
@@ -2208,43 +2222,46 @@
       <c r="J28" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
+      <c r="K28" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A29" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="4">
         <v>0.87557603686635899</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="4">
         <v>10</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="4">
         <v>27</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="4">
         <v>180</v>
       </c>
-      <c r="F29">
-        <v>0</v>
-      </c>
-      <c r="G29">
+      <c r="F29" s="4">
+        <v>0</v>
+      </c>
+      <c r="G29" s="4">
         <v>0.27027027027027001</v>
       </c>
-      <c r="H29">
-        <v>1</v>
-      </c>
-      <c r="I29">
+      <c r="H29" s="4">
+        <v>1</v>
+      </c>
+      <c r="I29" s="4">
         <v>0.42553191489361702</v>
       </c>
-      <c r="J29" t="s">
+      <c r="J29" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="K29" s="1" t="s">
+      <c r="K29" s="4" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>69</v>
       </c>
@@ -2275,145 +2292,151 @@
       <c r="J30" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
+      <c r="K30" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A31" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="4">
         <v>0.99025341130604205</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="4">
         <v>4</v>
       </c>
-      <c r="D31">
-        <v>0</v>
-      </c>
-      <c r="E31">
+      <c r="D31" s="4">
+        <v>0</v>
+      </c>
+      <c r="E31" s="4">
         <v>504</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="4">
         <v>5</v>
       </c>
-      <c r="G31">
-        <v>1</v>
-      </c>
-      <c r="H31">
+      <c r="G31" s="4">
+        <v>1</v>
+      </c>
+      <c r="H31" s="4">
         <v>0.44444444444444398</v>
       </c>
-      <c r="I31">
+      <c r="I31" s="4">
         <v>0.61538461538461497</v>
       </c>
-      <c r="J31" t="s">
+      <c r="J31" s="4" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
+      <c r="K31" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A32" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="4">
         <v>0.98536585365853602</v>
       </c>
-      <c r="C32">
-        <v>0</v>
-      </c>
-      <c r="D32">
-        <v>0</v>
-      </c>
-      <c r="E32">
+      <c r="C32" s="4">
+        <v>0</v>
+      </c>
+      <c r="D32" s="4">
+        <v>0</v>
+      </c>
+      <c r="E32" s="4">
         <v>606</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="4">
         <v>9</v>
       </c>
-      <c r="G32" t="s">
-        <v>21</v>
-      </c>
-      <c r="H32" t="s">
-        <v>21</v>
-      </c>
-      <c r="I32" t="s">
-        <v>21</v>
-      </c>
-      <c r="J32" t="s">
+      <c r="G32" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I32" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J32" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="K32" s="1" t="s">
+      <c r="K32" s="4" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
+    <row r="33" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A33" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="2">
         <v>0.97663551401869098</v>
       </c>
-      <c r="C33">
-        <v>0</v>
-      </c>
-      <c r="D33">
-        <v>0</v>
-      </c>
-      <c r="E33">
+      <c r="C33" s="2">
+        <v>0</v>
+      </c>
+      <c r="D33" s="2">
+        <v>0</v>
+      </c>
+      <c r="E33" s="2">
         <v>418</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="2">
         <v>10</v>
       </c>
-      <c r="G33" t="s">
-        <v>21</v>
-      </c>
-      <c r="H33" t="s">
-        <v>21</v>
-      </c>
-      <c r="I33" t="s">
-        <v>21</v>
-      </c>
-      <c r="J33" t="s">
+      <c r="G33" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J33" s="2" t="s">
         <v>94</v>
       </c>
       <c r="K33" s="2" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
+    <row r="34" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A34" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="4">
         <v>0.99760191846522694</v>
       </c>
-      <c r="C34">
-        <v>0</v>
-      </c>
-      <c r="D34">
-        <v>0</v>
-      </c>
-      <c r="E34">
+      <c r="C34" s="4">
+        <v>0</v>
+      </c>
+      <c r="D34" s="4">
+        <v>0</v>
+      </c>
+      <c r="E34" s="4">
         <v>1248</v>
       </c>
-      <c r="F34">
+      <c r="F34" s="4">
         <v>3</v>
       </c>
-      <c r="G34" t="s">
-        <v>21</v>
-      </c>
-      <c r="H34" t="s">
-        <v>21</v>
-      </c>
-      <c r="I34" t="s">
-        <v>21</v>
-      </c>
-      <c r="J34" t="s">
+      <c r="G34" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I34" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J34" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="K34" s="1" t="s">
+      <c r="K34" s="4" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>56</v>
       </c>
@@ -2445,7 +2468,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>68</v>
       </c>
@@ -2480,7 +2503,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>72</v>
       </c>
@@ -2515,7 +2538,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>39</v>
       </c>
@@ -2550,7 +2573,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>40</v>
       </c>
@@ -2585,7 +2608,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>37</v>
       </c>
@@ -2617,7 +2640,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>44</v>
       </c>
@@ -2649,7 +2672,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>48</v>
       </c>
@@ -2681,7 +2704,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>35</v>
       </c>
@@ -2710,7 +2733,7 @@
         <v>0.66666666666666596</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -2739,7 +2762,7 @@
         <v>0.66666666666666596</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>70</v>
       </c>
@@ -2768,7 +2791,7 @@
         <v>0.66666666666666596</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>85</v>
       </c>
@@ -2797,7 +2820,7 @@
         <v>0.68965517241379304</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>54</v>
       </c>
@@ -2826,7 +2849,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>25</v>
       </c>
@@ -2855,7 +2878,7 @@
         <v>0.71428571428571397</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>9</v>
       </c>
@@ -2884,7 +2907,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>87</v>
       </c>
@@ -2913,7 +2936,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>86</v>
       </c>
@@ -2942,7 +2965,7 @@
         <v>0.76923076923076905</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -2971,7 +2994,7 @@
         <v>0.79120879120879095</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>15</v>
       </c>
@@ -3000,7 +3023,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>47</v>
       </c>
@@ -3029,7 +3052,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>88</v>
       </c>
@@ -3058,7 +3081,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>28</v>
       </c>
@@ -3087,7 +3110,7 @@
         <v>0.81818181818181801</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>55</v>
       </c>
@@ -3116,7 +3139,7 @@
         <v>0.81818181818181801</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>61</v>
       </c>
@@ -3145,7 +3168,7 @@
         <v>0.81818181818181801</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>74</v>
       </c>
@@ -3174,7 +3197,7 @@
         <v>0.82352941176470495</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
         <v>10</v>
       </c>
@@ -3203,7 +3226,7 @@
         <v>0.83333333333333304</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
         <v>71</v>
       </c>
@@ -3232,7 +3255,7 @@
         <v>0.85714285714285698</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
         <v>90</v>
       </c>
@@ -3261,7 +3284,7 @@
         <v>0.85714285714285698</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
         <v>50</v>
       </c>
@@ -3290,7 +3313,7 @@
         <v>0.86538461538461497</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
         <v>53</v>
       </c>
@@ -3319,7 +3342,7 @@
         <v>0.86842105263157798</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>57</v>
       </c>
@@ -3348,7 +3371,7 @@
         <v>0.86956521739130399</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
         <v>12</v>
       </c>
@@ -3377,7 +3400,7 @@
         <v>0.88721804511278102</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
         <v>46</v>
       </c>
@@ -3406,7 +3429,7 @@
         <v>0.88888888888888895</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>60</v>
       </c>
@@ -3435,7 +3458,7 @@
         <v>0.89655172413793105</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
         <v>14</v>
       </c>
@@ -3464,7 +3487,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
         <v>64</v>
       </c>
@@ -3493,7 +3516,7 @@
         <v>0.93333333333333302</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
         <v>75</v>
       </c>
@@ -3522,7 +3545,7 @@
         <v>0.93333333333333302</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
         <v>31</v>
       </c>
@@ -3551,7 +3574,7 @@
         <v>0.94736842105263097</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
         <v>62</v>
       </c>
@@ -3580,7 +3603,7 @@
         <v>0.952380952380952</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
         <v>63</v>
       </c>
@@ -3609,7 +3632,7 @@
         <v>0.952380952380952</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
         <v>65</v>
       </c>
@@ -3638,7 +3661,7 @@
         <v>0.952380952380952</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
         <v>67</v>
       </c>
@@ -3667,7 +3690,7 @@
         <v>0.952380952380952</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
         <v>16</v>
       </c>
@@ -3696,7 +3719,7 @@
         <v>0.96428571428571397</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
         <v>19</v>
       </c>
@@ -3725,7 +3748,7 @@
         <v>0.967741935483871</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
         <v>17</v>
       </c>
@@ -3754,7 +3777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
         <v>18</v>
       </c>
@@ -3783,7 +3806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
         <v>27</v>
       </c>
@@ -3812,7 +3835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
         <v>66</v>
       </c>

</xml_diff>